<commit_message>
Added names to the stories
</commit_message>
<xml_diff>
--- a/Stories.xlsx
+++ b/Stories.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\koob8\Documents\ScreenManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{031F9942-EC43-420C-BF5F-CCAAB9341F38}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28111236-0621-4B86-8AD9-14666887CDEF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{23E1906B-1CE6-414F-8235-72A9FA54ED2A}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Week 1 Stories Table</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>Time Estimate (Hrs)</t>
+  </si>
+  <si>
+    <t>Matt Peter, Michael Riess, Jonah Kubath</t>
   </si>
 </sst>
 </file>
@@ -424,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B18C7E13-27B9-4F26-BFB6-6B0C8DF0D2D8}">
-  <dimension ref="A2:E11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,6 +442,11 @@
     <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+    </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>

</xml_diff>